<commit_message>
Movies URL generator code added
</commit_message>
<xml_diff>
--- a/Arabic/Movies.xlsx
+++ b/Arabic/Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeromedoss.a\Desktop\GitMovie\LetzzWatch\Arabic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{412B6C4F-9934-4C20-A127-5024E9DB2A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE7DBFA-84BE-488C-B279-900EA2785434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2196" yWindow="204" windowWidth="12540" windowHeight="12036" xr2:uid="{D98FB0A1-97CA-467D-B0FD-6E561E60A7A1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>S.no</t>
   </si>
@@ -45,6 +45,24 @@
   </si>
   <si>
     <t>Movie link</t>
+  </si>
+  <si>
+    <t>The Matchmaker</t>
+  </si>
+  <si>
+    <t>Under the Fig Trees</t>
+  </si>
+  <si>
+    <t>The Blue Whale</t>
+  </si>
+  <si>
+    <t>The Worthy</t>
+  </si>
+  <si>
+    <t>The Land</t>
+  </si>
+  <si>
+    <t>The Ambush</t>
   </si>
 </sst>
 </file>
@@ -396,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF81475-ED37-4FD3-B5E0-2B639D4607E5}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,7 +437,56 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>